<commit_message>
Added tests to be done with priority
</commit_message>
<xml_diff>
--- a/testInfo.xlsx
+++ b/testInfo.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="276">
   <si>
     <t xml:space="preserve">Testname </t>
   </si>
@@ -904,6 +904,12 @@
   </si>
   <si>
     <t>Multi-Kernel system with diluted and other kernel as per Pons et al.</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>Deeper Models</t>
   </si>
 </sst>
 </file>
@@ -8929,10 +8935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9570,7 +9576,9 @@
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
+      <c r="E33" s="38" t="s">
+        <v>274</v>
+      </c>
       <c r="F33" s="38"/>
       <c r="G33" s="65"/>
       <c r="H33" s="38"/>
@@ -9580,7 +9588,9 @@
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
+      <c r="E34" s="38" t="s">
+        <v>274</v>
+      </c>
       <c r="F34" s="38"/>
       <c r="G34" s="65"/>
       <c r="H34" s="38"/>
@@ -9590,7 +9600,9 @@
       <c r="B35" s="38"/>
       <c r="C35" s="38"/>
       <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
+      <c r="E35" s="38" t="s">
+        <v>274</v>
+      </c>
       <c r="F35" s="38"/>
       <c r="G35" s="65"/>
       <c r="H35" s="38"/>
@@ -9610,7 +9622,9 @@
       <c r="B37" s="38"/>
       <c r="C37" s="38"/>
       <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
+      <c r="E37" s="38" t="s">
+        <v>275</v>
+      </c>
       <c r="F37" s="38"/>
       <c r="G37" s="65"/>
       <c r="H37" s="38"/>
@@ -9620,7 +9634,9 @@
       <c r="B38" s="38"/>
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
+      <c r="E38" s="38" t="s">
+        <v>274</v>
+      </c>
       <c r="F38" s="38"/>
       <c r="G38" s="65"/>
       <c r="H38" s="38"/>
@@ -9630,7 +9646,9 @@
       <c r="B39" s="38"/>
       <c r="C39" s="38"/>
       <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
+      <c r="E39" s="38" t="s">
+        <v>274</v>
+      </c>
       <c r="F39" s="38"/>
       <c r="G39" s="65"/>
       <c r="H39" s="38"/>
@@ -9640,7 +9658,9 @@
       <c r="B40" s="38"/>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
+      <c r="E40" s="38" t="s">
+        <v>274</v>
+      </c>
       <c r="F40" s="38"/>
       <c r="G40" s="65"/>
       <c r="H40" s="38"/>
@@ -9713,9 +9733,16 @@
       <c r="E47" s="38"/>
       <c r="F47" s="38"/>
       <c r="G47" s="65"/>
+      <c r="H47" s="38"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G48" s="66"/>
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="65"/>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G49" s="66"/>
@@ -9740,6 +9767,9 @@
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G56" s="66"/>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>